<commit_message>
Update data and automatic last updated date
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartm\Documents\GitHub\Stock-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8534C34C-E170-4A63-BD69-1CC1D96F59C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEEEE5D-3E95-4916-80A9-48F69203A7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29A6A1C3-F615-434C-B187-5E0D3705EC97}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -200,6 +200,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -289,13 +290,13 @@
             <v>12842.73</v>
           </cell>
           <cell r="U5">
-            <v>36613.819000000003</v>
+            <v>36634.853000000003</v>
           </cell>
           <cell r="V5">
             <v>1706</v>
           </cell>
           <cell r="X5">
-            <v>51162.548999999999</v>
+            <v>51183.582999999999</v>
           </cell>
         </row>
         <row r="6">
@@ -303,13 +304,13 @@
             <v>19345.87</v>
           </cell>
           <cell r="U6">
-            <v>1879.0670000000002</v>
+            <v>1879.2190000000003</v>
           </cell>
           <cell r="W6">
             <v>8824.8799999999992</v>
           </cell>
           <cell r="X6">
-            <v>30049.816999999995</v>
+            <v>30049.968999999997</v>
           </cell>
         </row>
       </sheetData>
@@ -444,25 +445,25 @@
     <v>4</v>
     <v>96.7</v>
     <v>73.69</v>
-    <v>0.57499999999999996</v>
-    <v>6.1339999999999997E-3</v>
+    <v>0.63500000000000001</v>
+    <v>6.7739999999999996E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>2E-3</v>
     <v>94.43</v>
     <v>ETF</v>
-    <v>45502.385162037041</v>
+    <v>45502.399131944447</v>
     <v>0</v>
     <v>94.12</v>
     <v>76531170531.970001</v>
     <v>iShs CoreMSCI Wld ETF USD A</v>
     <v>94.375</v>
     <v>93.745000000000005</v>
-    <v>94.32</v>
+    <v>94.38</v>
     <v>IWDA</v>
     <v>iShs CoreMSCI Wld ETF USD A (XAMS:IWDA)</v>
-    <v>37286</v>
+    <v>38157</v>
   </rv>
   <rv s="2">
     <v>1</v>
@@ -485,25 +486,25 @@
     <v>4</v>
     <v>32.82</v>
     <v>26.53</v>
-    <v>0.154</v>
-    <v>4.9090000000000002E-3</v>
+    <v>0.16500000000000001</v>
+    <v>5.2599999999999999E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>1.8E-3</v>
     <v>31.565999999999999</v>
     <v>ETF</v>
-    <v>45502.38517361111</v>
+    <v>45502.399155092593</v>
     <v>3</v>
     <v>31.5</v>
     <v>20540937542.860001</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA</v>
     <v>31.550999999999998</v>
     <v>31.369</v>
-    <v>31.523</v>
+    <v>31.533999999999999</v>
     <v>EMIM</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA (XAMS:EMIM)</v>
-    <v>10521</v>
+    <v>10805</v>
   </rv>
   <rv s="2">
     <v>4</v>
@@ -530,7 +531,7 @@
     <v>2.2000000000000001E-3</v>
     <v>122.298</v>
     <v>ETF</v>
-    <v>45502.385162037041</v>
+    <v>45502.399131944447</v>
     <v>121.9</v>
     <v>12527969851.459999</v>
     <v>FTSE AllWld UCITS ETF USD A</v>
@@ -1161,18 +1162,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B5A40D-BB52-45F6-9C73-EDE2E7F2B2C7}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>[1]Assets!$B$6</f>
         <v>IWDA</v>
@@ -1221,18 +1223,18 @@
       </c>
       <c r="E2" s="4" cm="1">
         <f t="array" ref="E2">_FV(O3,"Price")</f>
-        <v>94.32</v>
+        <v>94.38</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2">
         <f>[1]Ledger!$X$5</f>
-        <v>51162.548999999999</v>
+        <v>51183.582999999999</v>
       </c>
       <c r="H2">
         <f>[1]Ledger!$U$5</f>
-        <v>36613.819000000003</v>
+        <v>36634.853000000003</v>
       </c>
       <c r="I2">
         <f>[1]Ledger!$T$5</f>
@@ -1243,7 +1245,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>[1]Assets!$B$7</f>
         <v>EMIM</v>
@@ -1262,18 +1264,18 @@
       </c>
       <c r="E3" s="5" cm="1">
         <f t="array" ref="E3">_FV(O4,"Price")</f>
-        <v>31.523</v>
+        <v>31.533999999999999</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3">
         <f>[1]Ledger!$X$6</f>
-        <v>30049.816999999995</v>
+        <v>30049.968999999997</v>
       </c>
       <c r="H3">
         <f>[1]Ledger!$U$6</f>
-        <v>1879.0670000000002</v>
+        <v>1879.2190000000003</v>
       </c>
       <c r="I3">
         <f>[1]Ledger!$T$6</f>
@@ -1286,8 +1288,12 @@
       <c r="O3" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
+      <c r="U3" s="7">
+        <f ca="1">TODAY()</f>
+        <v>45502</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>[1]Assets!$B$8</f>
         <v>VWCE</v>
@@ -1312,12 +1318,12 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O5" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M12" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
show datetime in footer
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartm\Documents\GitHub\Stock-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B21821-B7CC-4DCB-BE06-67E68F168471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA4FDE-53CE-4B1E-8BC4-15E8CA4D489F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="3180" windowWidth="24480" windowHeight="13185" xr2:uid="{29A6A1C3-F615-434C-B187-5E0D3705EC97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29A6A1C3-F615-434C-B187-5E0D3705EC97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,10 +197,10 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -290,13 +290,13 @@
             <v>12842.73</v>
           </cell>
           <cell r="U5">
-            <v>36582.455000000002</v>
+            <v>36619.404000000002</v>
           </cell>
           <cell r="V5">
             <v>1706</v>
           </cell>
           <cell r="X5">
-            <v>51131.184999999998</v>
+            <v>51168.134000000005</v>
           </cell>
         </row>
         <row r="6">
@@ -304,13 +304,13 @@
             <v>19345.87</v>
           </cell>
           <cell r="U6">
-            <v>1878.5130000000001</v>
+            <v>1879.5290000000002</v>
           </cell>
           <cell r="W6">
             <v>8824.8799999999992</v>
           </cell>
           <cell r="X6">
-            <v>30049.262999999999</v>
+            <v>30050.278999999995</v>
           </cell>
         </row>
       </sheetData>
@@ -445,25 +445,25 @@
     <v>4</v>
     <v>96.7</v>
     <v>73.69</v>
-    <v>0.31</v>
-    <v>3.3010000000000001E-3</v>
+    <v>0.44</v>
+    <v>4.6849999999999999E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>2E-3</v>
     <v>94.394999999999996</v>
     <v>ETF</v>
-    <v>45503.39303240741</v>
+    <v>45503.491944444446</v>
     <v>0</v>
-    <v>94.16</v>
+    <v>94.15</v>
     <v>76531170531.970001</v>
     <v>iShs CoreMSCI Wld ETF USD A</v>
     <v>94.265000000000001</v>
     <v>93.92</v>
-    <v>94.23</v>
+    <v>94.36</v>
     <v>IWDA</v>
     <v>iShs CoreMSCI Wld ETF USD A (XAMS:IWDA)</v>
-    <v>35111</v>
+    <v>43347</v>
   </rv>
   <rv s="2">
     <v>1</v>
@@ -486,25 +486,25 @@
     <v>4</v>
     <v>32.82</v>
     <v>26.53</v>
-    <v>0.14099999999999999</v>
-    <v>4.4979999999999994E-3</v>
+    <v>0.16800000000000001</v>
+    <v>5.3600000000000002E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>1.8E-3</v>
-    <v>31.506</v>
+    <v>31.512</v>
     <v>ETF</v>
-    <v>45503.393067129633</v>
+    <v>45503.491944444446</v>
     <v>3</v>
-    <v>31.460999999999999</v>
+    <v>31.43</v>
     <v>20540937542.860001</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA</v>
     <v>31.462</v>
     <v>31.344000000000001</v>
-    <v>31.484999999999999</v>
+    <v>31.512</v>
     <v>EMIM</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA (XAMS:EMIM)</v>
-    <v>16269</v>
+    <v>17324</v>
   </rv>
   <rv s="2">
     <v>4</v>
@@ -527,25 +527,25 @@
     <v>4</v>
     <v>125.14</v>
     <v>96.52</v>
-    <v>0.42</v>
-    <v>3.4560000000000003E-3</v>
+    <v>0.57999999999999996</v>
+    <v>4.7720000000000002E-3</v>
     <v>EUR</v>
     <v>Xetra</v>
     <v>XETR</v>
     <v>2.2000000000000001E-3</v>
     <v>122.14</v>
     <v>ETF</v>
-    <v>45503.392893518518</v>
+    <v>45503.491840277777</v>
     <v>6</v>
-    <v>121.84</v>
+    <v>121.82</v>
     <v>12527969851.459999</v>
     <v>FTSE AllWld UCITS ETF USD A</v>
     <v>121.98</v>
     <v>121.54</v>
-    <v>121.96</v>
+    <v>122.12</v>
     <v>VWCE</v>
     <v>FTSE AllWld UCITS ETF USD A (XETR:VWCE)</v>
-    <v>19599</v>
+    <v>31380</v>
   </rv>
   <rv s="2">
     <v>7</v>
@@ -1088,13 +1088,13 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="15.7109375" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1113,10 +1113,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1146,18 +1146,18 @@
       </c>
       <c r="E2" s="4" cm="1">
         <f t="array" ref="E2">_FV(O3,"Price")</f>
-        <v>94.23</v>
+        <v>94.36</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2">
         <f>[1]Ledger!$X$5</f>
-        <v>51131.184999999998</v>
+        <v>51168.134000000005</v>
       </c>
       <c r="H2">
         <f>[1]Ledger!$U$5</f>
-        <v>36582.455000000002</v>
+        <v>36619.404000000002</v>
       </c>
       <c r="I2">
         <f>[1]Ledger!$T$5</f>
@@ -1187,18 +1187,18 @@
       </c>
       <c r="E3" s="5" cm="1">
         <f t="array" ref="E3">_FV(O4,"Price")</f>
-        <v>31.484999999999999</v>
+        <v>31.512</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3">
         <f>[1]Ledger!$X$6</f>
-        <v>30049.262999999999</v>
+        <v>30050.278999999995</v>
       </c>
       <c r="H3">
         <f>[1]Ledger!$U$6</f>
-        <v>1878.5130000000001</v>
+        <v>1879.5290000000002</v>
       </c>
       <c r="I3">
         <f>[1]Ledger!$T$6</f>
@@ -1211,9 +1211,9 @@
       <c r="O3" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="U3" s="6">
-        <f ca="1">TODAY()</f>
-        <v>45503</v>
+      <c r="U3" s="7">
+        <f ca="1">NOW()</f>
+        <v>45503.585826273149</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="E4" s="4" cm="1">
         <f t="array" ref="E4">_FV(O5,"Price")</f>
-        <v>121.96</v>
+        <v>122.12</v>
       </c>
       <c r="O4" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1245,6 +1245,7 @@
       <c r="O5" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
+      <c r="U5" s="7"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M12" s="5"/>

</xml_diff>

<commit_message>
refacter/cleanup of code; group digitz and localized formating
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartm\Documents\GitHub\Stock-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA4FDE-53CE-4B1E-8BC4-15E8CA4D489F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A05898-BBA9-4C35-98D1-BAE38B4841F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29A6A1C3-F615-434C-B187-5E0D3705EC97}"/>
   </bookViews>
@@ -197,10 +197,10 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -290,13 +290,13 @@
             <v>12842.73</v>
           </cell>
           <cell r="U5">
-            <v>36619.404000000002</v>
+            <v>36691.686000000002</v>
           </cell>
           <cell r="V5">
             <v>1706</v>
           </cell>
           <cell r="X5">
-            <v>51168.134000000005</v>
+            <v>51240.415999999997</v>
           </cell>
         </row>
         <row r="6">
@@ -304,13 +304,13 @@
             <v>19345.87</v>
           </cell>
           <cell r="U6">
-            <v>1879.5290000000002</v>
+            <v>1884.1340000000002</v>
           </cell>
           <cell r="W6">
             <v>8824.8799999999992</v>
           </cell>
           <cell r="X6">
-            <v>30050.278999999995</v>
+            <v>30054.883999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -445,25 +445,25 @@
     <v>4</v>
     <v>96.7</v>
     <v>73.69</v>
-    <v>0.44</v>
-    <v>4.6849999999999999E-3</v>
+    <v>0.65</v>
+    <v>6.9210000000000001E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>2E-3</v>
-    <v>94.394999999999996</v>
+    <v>94.7</v>
     <v>ETF</v>
-    <v>45503.491944444446</v>
+    <v>45503.582280092596</v>
     <v>0</v>
     <v>94.15</v>
     <v>76531170531.970001</v>
     <v>iShs CoreMSCI Wld ETF USD A</v>
     <v>94.265000000000001</v>
     <v>93.92</v>
-    <v>94.36</v>
+    <v>94.57</v>
     <v>IWDA</v>
     <v>iShs CoreMSCI Wld ETF USD A (XAMS:IWDA)</v>
-    <v>43347</v>
+    <v>57018</v>
   </rv>
   <rv s="2">
     <v>1</v>
@@ -486,25 +486,25 @@
     <v>4</v>
     <v>32.82</v>
     <v>26.53</v>
-    <v>0.16800000000000001</v>
-    <v>5.3600000000000002E-3</v>
+    <v>0.128</v>
+    <v>4.084E-3</v>
     <v>EUR</v>
     <v>Euronext Amsterdam</v>
     <v>XAMS</v>
     <v>1.8E-3</v>
-    <v>31.512</v>
+    <v>31.532</v>
     <v>ETF</v>
-    <v>45503.491944444446</v>
+    <v>45503.582280092596</v>
     <v>3</v>
     <v>31.43</v>
     <v>20540937542.860001</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA</v>
     <v>31.462</v>
     <v>31.344000000000001</v>
-    <v>31.512</v>
+    <v>31.472000000000001</v>
     <v>EMIM</v>
     <v>iShs CrMSCI EMIMIUCITS ETFUSDA (XAMS:EMIM)</v>
-    <v>17324</v>
+    <v>19002</v>
   </rv>
   <rv s="2">
     <v>4</v>
@@ -527,25 +527,25 @@
     <v>4</v>
     <v>125.14</v>
     <v>96.52</v>
-    <v>0.57999999999999996</v>
-    <v>4.7720000000000002E-3</v>
+    <v>0.8</v>
+    <v>6.5820000000000002E-3</v>
     <v>EUR</v>
     <v>Xetra</v>
     <v>XETR</v>
     <v>2.2000000000000001E-3</v>
-    <v>122.14</v>
+    <v>122.5</v>
     <v>ETF</v>
-    <v>45503.491840277777</v>
+    <v>45503.582280092596</v>
     <v>6</v>
     <v>121.82</v>
     <v>12527969851.459999</v>
     <v>FTSE AllWld UCITS ETF USD A</v>
     <v>121.98</v>
     <v>121.54</v>
-    <v>122.12</v>
+    <v>122.34</v>
     <v>VWCE</v>
     <v>FTSE AllWld UCITS ETF USD A (XETR:VWCE)</v>
-    <v>31380</v>
+    <v>45269</v>
   </rv>
   <rv s="2">
     <v>7</v>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,10 +1113,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1146,18 +1146,18 @@
       </c>
       <c r="E2" s="4" cm="1">
         <f t="array" ref="E2">_FV(O3,"Price")</f>
-        <v>94.36</v>
+        <v>94.57</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2">
         <f>[1]Ledger!$X$5</f>
-        <v>51168.134000000005</v>
+        <v>51240.415999999997</v>
       </c>
       <c r="H2">
         <f>[1]Ledger!$U$5</f>
-        <v>36619.404000000002</v>
+        <v>36691.686000000002</v>
       </c>
       <c r="I2">
         <f>[1]Ledger!$T$5</f>
@@ -1187,18 +1187,18 @@
       </c>
       <c r="E3" s="5" cm="1">
         <f t="array" ref="E3">_FV(O4,"Price")</f>
-        <v>31.512</v>
+        <v>31.472000000000001</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3">
         <f>[1]Ledger!$X$6</f>
-        <v>30050.278999999995</v>
+        <v>30054.883999999998</v>
       </c>
       <c r="H3">
         <f>[1]Ledger!$U$6</f>
-        <v>1879.5290000000002</v>
+        <v>1884.1340000000002</v>
       </c>
       <c r="I3">
         <f>[1]Ledger!$T$6</f>
@@ -1211,9 +1211,9 @@
       <c r="O3" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="6">
         <f ca="1">NOW()</f>
-        <v>45503.585826273149</v>
+        <v>45503.676063194442</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="E4" s="4" cm="1">
         <f t="array" ref="E4">_FV(O5,"Price")</f>
-        <v>122.12</v>
+        <v>122.34</v>
       </c>
       <c r="O4" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1245,7 +1245,7 @@
       <c r="O5" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="U5" s="7"/>
+      <c r="U5" s="6"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M12" s="5"/>

</xml_diff>